<commit_message>
Programa com Janela - Usando o flet - 02-09-25
</commit_message>
<xml_diff>
--- a/banco_conexao/01_crud_uma_entidade/planilhas_exportadas/pessoas.xlsx
+++ b/banco_conexao/01_crud_uma_entidade/planilhas_exportadas/pessoas.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -815,6 +815,46 @@
         </is>
       </c>
     </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>20</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Pandas</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>panda@panda.com.br</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>01/01/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>21</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Pandas Da Silva</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>pandassilva@gmail.com</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>01/01/2010</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>